<commit_message>
filter excel worksheet tab label update
</commit_message>
<xml_diff>
--- a/dependencies/bi/salmonella/heidelberg-SL476/script_dependents/script2/Filtered_Regions.xlsx
+++ b/dependencies/bi/salmonella/heidelberg-SL476/script_dependents/script2/Filtered_Regions.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/root/TStuber/Results/bi/salmonella/vsnp/heidelberg-SL476/script_dependents/script2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{FE1368A5-4C75-0544-A9E9-04EEF58C2F0A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{21FDAD08-0B7D-CE43-83B8-A2C8C599D016}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31480" yWindow="11140" windowWidth="18520" windowHeight="16740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="NC_016856.1" sheetId="2" r:id="rId1"/>
+    <sheet name="NC_011083.1" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>heidelberg-01</t>
   </si>
@@ -1440,7 +1440,7 @@
   <dimension ref="A1:B117"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>